<commit_message>
deploy new xlsx in middle of August v2
</commit_message>
<xml_diff>
--- a/src/data/locations.xlsx
+++ b/src/data/locations.xlsx
@@ -8399,553 +8399,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="215">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="137">
     <dxf>
       <fill>
         <patternFill>
@@ -10233,8 +9687,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AD745"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A680" zoomScale="116" workbookViewId="0">
-      <selection activeCell="J753" sqref="J753"/>
+    <sheetView tabSelected="1" topLeftCell="A503" zoomScale="116" workbookViewId="0">
+      <selection activeCell="J580" sqref="J580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23825,7 +23279,7 @@
         <v>988</v>
       </c>
       <c r="B194" s="4" t="str">
-        <f t="shared" ref="B194:B257" si="3">TEXT(C194, "mm/dd/yyy")</f>
+        <f t="shared" ref="B194:B238" si="3">TEXT(C194, "mm/dd/yyy")</f>
         <v>05/05/2018</v>
       </c>
       <c r="C194" s="5">
@@ -43581,7 +43035,7 @@
         <v>2323</v>
       </c>
       <c r="B496" s="4" t="str">
-        <f t="shared" ref="B496:B559" si="8">TEXT(C496, "mm/dd/yyy")</f>
+        <f t="shared" ref="B496:B552" si="8">TEXT(C496, "mm/dd/yyy")</f>
         <v>07/13/2018</v>
       </c>
       <c r="C496" s="10">
@@ -48991,8 +48445,8 @@
         <v>1911</v>
       </c>
       <c r="I580" s="13"/>
-      <c r="J580" s="13" t="s">
-        <v>438</v>
+      <c r="J580" s="46" t="s">
+        <v>3</v>
       </c>
       <c r="K580" s="13" t="s">
         <v>4</v>
@@ -57888,7 +57342,7 @@
         <v>2576</v>
       </c>
       <c r="B717" s="4" t="str">
-        <f t="shared" ref="B717:B748" si="14">TEXT(C717, "mm/dd/yyy")</f>
+        <f t="shared" ref="B717:B745" si="14">TEXT(C717, "mm/dd/yyy")</f>
         <v>09/07/2018</v>
       </c>
       <c r="C717" s="5">
@@ -59780,499 +59234,499 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="J128">
-    <cfRule type="containsText" dxfId="214" priority="121" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="136" priority="121" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="122" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="135" priority="122" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J128)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="123" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="134" priority="123" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J128)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J130">
-    <cfRule type="containsText" dxfId="211" priority="115" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="133" priority="115" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J130)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="116" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="132" priority="116" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J130)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="117" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="131" priority="117" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J130)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J133">
-    <cfRule type="containsText" dxfId="208" priority="106" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="130" priority="106" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J133)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="107" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="129" priority="107" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J133)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="108" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="128" priority="108" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J133)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J144">
-    <cfRule type="containsText" dxfId="205" priority="103" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="127" priority="103" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="104" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="126" priority="104" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="105" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="125" priority="105" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J148">
-    <cfRule type="containsText" dxfId="202" priority="91" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="124" priority="91" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J148)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="92" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="123" priority="92" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J148)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="93" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="122" priority="93" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J148)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J311">
-    <cfRule type="containsText" dxfId="199" priority="37" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="121" priority="37" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J311)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="38" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="120" priority="38" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J311)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="39" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="119" priority="39" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J311)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J546:J613 J619:J625 J627:J703 J705:J745">
-    <cfRule type="containsText" dxfId="196" priority="31" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="118" priority="31" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J546)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="32" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="117" priority="32" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J546)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="33" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="116" priority="33" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J546)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J163:J177">
-    <cfRule type="containsText" dxfId="193" priority="127" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="115" priority="127" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="128" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="114" priority="128" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J163)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="129" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="113" priority="129" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J163)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127">
-    <cfRule type="containsText" dxfId="190" priority="124" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="112" priority="124" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="125" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="111" priority="125" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J127)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="126" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="110" priority="126" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J129">
-    <cfRule type="containsText" dxfId="187" priority="118" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="109" priority="118" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J129)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="119" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="108" priority="119" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J129)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="120" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="107" priority="120" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J129)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J131">
-    <cfRule type="containsText" dxfId="184" priority="112" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="106" priority="112" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J131)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="113" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="105" priority="113" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J131)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="114" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="104" priority="114" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J132">
-    <cfRule type="containsText" dxfId="181" priority="109" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="103" priority="109" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J132)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="110" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="102" priority="110" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J132)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="111" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="101" priority="111" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J145">
-    <cfRule type="containsText" dxfId="178" priority="100" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="100" priority="100" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="101" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="99" priority="101" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J145)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="102" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="98" priority="102" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J145)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J146">
-    <cfRule type="containsText" dxfId="175" priority="97" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="97" priority="97" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="98" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="96" priority="98" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J146)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="99" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="95" priority="99" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J147">
-    <cfRule type="containsText" dxfId="172" priority="94" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="94" priority="94" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J147)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="95" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="93" priority="95" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J147)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="96" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="92" priority="96" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J147)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J149">
-    <cfRule type="containsText" dxfId="169" priority="88" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="91" priority="88" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="89" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="90" priority="89" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="90" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J150">
-    <cfRule type="containsText" dxfId="166" priority="85" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="88" priority="85" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="86" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="87" priority="86" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J150)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="87" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J150)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J151">
-    <cfRule type="containsText" dxfId="163" priority="82" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="85" priority="82" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="83" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="84" priority="83" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J151)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="84" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J151)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J152">
-    <cfRule type="containsText" dxfId="160" priority="79" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="82" priority="79" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="80" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J152)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="81" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J152)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J153">
-    <cfRule type="containsText" dxfId="157" priority="76" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="79" priority="76" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="77" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J153)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="78" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J153)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J154">
-    <cfRule type="containsText" dxfId="154" priority="73" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="76" priority="73" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="74" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="75" priority="74" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J154)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="75" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J154)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J155">
-    <cfRule type="containsText" dxfId="151" priority="70" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="73" priority="70" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="71" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="72" priority="71" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J155)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="72" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J155)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J156">
-    <cfRule type="containsText" dxfId="148" priority="67" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="70" priority="67" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="68" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="69" priority="68" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="69" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J157">
-    <cfRule type="containsText" dxfId="145" priority="64" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="67" priority="64" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="65" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J157)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="66" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J157)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J158">
-    <cfRule type="containsText" dxfId="142" priority="61" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="64" priority="61" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="62" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J158)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="63" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J158)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J159">
-    <cfRule type="containsText" dxfId="139" priority="58" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="61" priority="58" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="59" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J159)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="60" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J159)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J160">
-    <cfRule type="containsText" dxfId="136" priority="55" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="58" priority="55" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="56" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J160)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J160)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J161">
-    <cfRule type="containsText" dxfId="133" priority="52" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="55" priority="52" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="53" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="54" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J162">
-    <cfRule type="containsText" dxfId="130" priority="49" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="52" priority="49" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="50" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="51" priority="50" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="51" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J162)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J214:J222">
-    <cfRule type="containsText" dxfId="127" priority="46" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="49" priority="46" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="47" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="48" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J223">
-    <cfRule type="containsText" dxfId="124" priority="43" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="46" priority="43" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="44" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="45" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J126 J178:J213 J224:J310 J312:J461">
-    <cfRule type="containsText" dxfId="121" priority="133" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="43" priority="133" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="134" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="42" priority="134" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="135" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="41" priority="135" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134:J143">
-    <cfRule type="containsText" dxfId="118" priority="130" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="40" priority="130" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="131" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="39" priority="131" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J134)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="132" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="38" priority="132" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J134)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I140">
-    <cfRule type="duplicateValues" dxfId="115" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I138">
-    <cfRule type="duplicateValues" dxfId="114" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I137">
-    <cfRule type="duplicateValues" dxfId="113" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J462:J476 J479:J502 J504:J545">
-    <cfRule type="containsText" dxfId="112" priority="34" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J462)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="35" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J462)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="36" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J462)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H745">
-    <cfRule type="duplicateValues" dxfId="109" priority="136"/>
-    <cfRule type="duplicateValues" dxfId="108" priority="137"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="136"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="137"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J477">
-    <cfRule type="containsText" dxfId="59" priority="28" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J477)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="29" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J477)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J478">
-    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J478)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J478)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J503">
-    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J503)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J503)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J503)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J614">
-    <cfRule type="containsText" dxfId="41" priority="19" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J614)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="20" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J614)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J614)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J615">
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J615)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J615)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="18" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J615)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J616">
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J616)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="14" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J616)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="15" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J616)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J617">
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J617)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J617)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J617)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J618">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J618)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J618)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J618)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J626">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J626)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J626)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J626)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J704">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="On-Hold">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="On-Hold">
       <formula>NOT(ISERROR(SEARCH("On-Hold",J704)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Setting">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Setting">
       <formula>NOT(ISERROR(SEARCH("Setting",J704)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",J704)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>